<commit_message>
Se agrega campo password a la tabla usuario para manejar inicialmente una autenticación local.
</commit_message>
<xml_diff>
--- a/03 - Base de datos/excel/02 - usuario.xlsx
+++ b/03 - Base de datos/excel/02 - usuario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Dropbox\Desarrollo de software\DuocUC\PTY4478 - Portafolio de título\Base de datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Software\Duoc\admtaller-bd\03 - Base de datos\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C1C7EB-709F-4C68-ABEA-C79AE6847E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36F7882-324B-41FA-9EE3-DC30F37913C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="98">
   <si>
     <t>tabla</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t>Fabián</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -649,23 +655,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF8A036-CB43-482B-A6BA-E6BCB1927713}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="E23" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="41.28515625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="39.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="50.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
+    <col min="4" max="6" width="41.28515625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="39.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="50.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +680,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -681,28 +688,31 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -710,21 +720,24 @@
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="2" t="str">
+      <c r="J3" s="2" t="str">
         <f>"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
 CHAR(9)&amp;$A$2&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;$B$2&amp;","&amp;CHAR(10)&amp;
@@ -733,7 +746,8 @@
 CHAR(9)&amp;$E$2&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;$F$2&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;$G$2&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;$H$2&amp;")"&amp;CHAR(10)&amp;
+CHAR(9)&amp;$H$2&amp;","&amp;CHAR(10)&amp;
+CHAR(9)&amp;$I$2&amp;")"&amp;CHAR(10)&amp;
 "values ("&amp;CHAR(10)&amp;
 CHAR(9)&amp;A3&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;"'"&amp;B3&amp;"',"&amp;CHAR(10)&amp;
@@ -741,11 +755,13 @@
 CHAR(9)&amp;"'"&amp;D3&amp;"',"&amp;CHAR(10)&amp;
 CHAR(9)&amp;"'"&amp;E3&amp;"',"&amp;CHAR(10)&amp;
 CHAR(9)&amp;"'"&amp;F3&amp;"',"&amp;CHAR(10)&amp;
-CHAR(9)&amp;G3&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;H3&amp;");"&amp;CHAR(10)</f>
-        <v xml:space="preserve">insert into usuario (
-	id_usuario,
-	login,
+CHAR(9)&amp;"'"&amp;G3&amp;"',"&amp;CHAR(10)&amp;
+CHAR(9)&amp;H3&amp;","&amp;CHAR(10)&amp;
+CHAR(9)&amp;I3&amp;");"&amp;CHAR(10)</f>
+        <v xml:space="preserve">insert into usuario (
+	id_usuario,
+	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -755,6 +771,7 @@
 values (
 	1,
 	'admin',
+	'None',
 	'Administrador',
 	'',
 	'del sistema',
@@ -764,7 +781,7 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -772,25 +789,28 @@
         <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="str">
-        <f t="shared" ref="I4:I24" si="0">"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="str">
+        <f t="shared" ref="J4:J24" si="0">"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
 CHAR(9)&amp;$A$2&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;$B$2&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;$C$2&amp;","&amp;CHAR(10)&amp;
@@ -798,7 +818,8 @@
 CHAR(9)&amp;$E$2&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;$F$2&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;$G$2&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;$H$2&amp;")"&amp;CHAR(10)&amp;
+CHAR(9)&amp;$H$2&amp;","&amp;CHAR(10)&amp;
+CHAR(9)&amp;$I$2&amp;")"&amp;CHAR(10)&amp;
 "values ("&amp;CHAR(10)&amp;
 CHAR(9)&amp;A4&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;"'"&amp;B4&amp;"',"&amp;CHAR(10)&amp;
@@ -806,11 +827,13 @@
 CHAR(9)&amp;"'"&amp;D4&amp;"',"&amp;CHAR(10)&amp;
 CHAR(9)&amp;"'"&amp;E4&amp;"',"&amp;CHAR(10)&amp;
 CHAR(9)&amp;"'"&amp;F4&amp;"',"&amp;CHAR(10)&amp;
-CHAR(9)&amp;G4&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;H4&amp;");"&amp;CHAR(10)</f>
-        <v xml:space="preserve">insert into usuario (
-	id_usuario,
-	login,
+CHAR(9)&amp;"'"&amp;G4&amp;"',"&amp;CHAR(10)&amp;
+CHAR(9)&amp;H4&amp;","&amp;CHAR(10)&amp;
+CHAR(9)&amp;I4&amp;");"&amp;CHAR(10)</f>
+        <v xml:space="preserve">insert into usuario (
+	id_usuario,
+	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -820,6 +843,7 @@
 values (
 	2,
 	'jmoya@duoc.cl',
+	'None',
 	'Moya',
 	'Plaza',
 	'Jéssica',
@@ -829,7 +853,7 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -837,28 +861,32 @@
         <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="1">
-        <v>2</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="str">
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -868,6 +896,7 @@
 values (
 	3,
 	'maalvarez@duoc.cl',
+	'None',
 	'Álvarez',
 	'Román',
 	'Marco',
@@ -877,7 +906,7 @@
 </v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -885,28 +914,32 @@
         <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="1">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2" t="str">
+      <c r="G6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -916,6 +949,7 @@
 values (
 	4,
 	'c.gonzalez6@profesor.duoc.cl',
+	'None',
 	'González',
 	'Figueroa',
 	'Cristian',
@@ -925,7 +959,7 @@
 </v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -933,28 +967,32 @@
         <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="1">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2" t="str">
+      <c r="G7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -964,6 +1002,7 @@
 values (
 	5,
 	'r.ceura@profesor.duoc.cl',
+	'None',
 	'Ceura',
 	'Vergara',
 	'Raúl',
@@ -973,7 +1012,7 @@
 </v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -981,28 +1020,32 @@
         <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="1">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2" t="str">
+      <c r="G8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1012,6 +1055,7 @@
 values (
 	6,
 	'hec.fonseca@profesor.duoc.cl',
+	'None',
 	'Fonseca',
 	'Castillo',
 	'Héctor',
@@ -1021,7 +1065,7 @@
 </v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1029,28 +1073,32 @@
         <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="1">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2" t="str">
+      <c r="G9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1060,6 +1108,7 @@
 values (
 	7,
 	'xi.castro@profesor.duoc.cl',
+	'None',
 	'Castro',
 	'Arancibia',
 	'Ximena',
@@ -1069,7 +1118,7 @@
 </v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1077,28 +1126,32 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="1">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2" t="str">
+      <c r="G10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1108,6 +1161,7 @@
 values (
 	8,
 	'c.valenzuelair@profesor.duoc.cl',
+	'None',
 	'Valenzuela',
 	'Irrazabal',
 	'Carolina',
@@ -1117,7 +1171,7 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1125,28 +1179,32 @@
         <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="1">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2" t="str">
+      <c r="G11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1156,6 +1214,7 @@
 values (
 	9,
 	'sa.navarret@profesor.duoc.cl',
+	'None',
 	'Navarrete',
 	'Bustamante',
 	'Sandra',
@@ -1165,7 +1224,7 @@
 </v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1173,28 +1232,32 @@
         <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G12" s="1">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3">
-        <v>1</v>
-      </c>
-      <c r="I12" s="2" t="str">
+      <c r="G12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1204,6 +1267,7 @@
 values (
 	10,
 	'fabi.arancibia@profesor.duoc.cl',
+	'None',
 	'Arancibia',
 	'Severino',
 	'Fabián',
@@ -1213,7 +1277,7 @@
 </v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1221,28 +1285,32 @@
         <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="1">
-        <v>2</v>
-      </c>
-      <c r="H13" s="3">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2" t="str">
+      <c r="G13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1252,6 +1320,7 @@
 values (
 	11,
 	'roci.guzman@profesor.duoc.cl',
+	'None',
 	'Guzmán',
 	'Acuña',
 	'Rocío',
@@ -1261,7 +1330,7 @@
 </v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1269,28 +1338,32 @@
         <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G14" s="1">
-        <v>2</v>
-      </c>
-      <c r="H14" s="3">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2" t="str">
+      <c r="G14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1300,6 +1373,7 @@
 values (
 	12,
 	'al.camposa@profesor.duoc.cl',
+	'None',
 	'Campos',
 	'Acuña',
 	'Alejandra',
@@ -1309,7 +1383,7 @@
 </v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1317,28 +1391,32 @@
         <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="1">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3">
-        <v>1</v>
-      </c>
-      <c r="I15" s="2" t="str">
+      <c r="G15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1348,6 +1426,7 @@
 values (
 	13,
 	'cr.madariagam@profesor.duoc.cl',
+	'None',
 	'Madariaga',
 	'Martínez',
 	'Cristian',
@@ -1357,7 +1436,7 @@
 </v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1365,28 +1444,32 @@
         <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="1">
-        <v>2</v>
-      </c>
-      <c r="H16" s="3">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2" t="str">
+      <c r="G16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1396,6 +1479,7 @@
 values (
 	14,
 	'i.inostroza@profesor.duoc.cl',
+	'None',
 	'Inostroza',
 	'Rodríguez',
 	'Isaac',
@@ -1405,7 +1489,7 @@
 </v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1413,28 +1497,32 @@
         <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="1">
-        <v>2</v>
-      </c>
-      <c r="H17" s="3">
-        <v>1</v>
-      </c>
-      <c r="I17" s="2" t="str">
+      <c r="G17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1444,6 +1532,7 @@
 values (
 	15,
 	'v.fuentealbav@profesor.duoc.cl',
+	'None',
 	'Fuentealva',
 	'Vargas',
 	'Víctor',
@@ -1453,7 +1542,7 @@
 </v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1461,28 +1550,32 @@
         <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="1">
-        <v>2</v>
-      </c>
-      <c r="H18" s="3">
-        <v>1</v>
-      </c>
-      <c r="I18" s="2" t="str">
+      <c r="G18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="1">
+        <v>2</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1492,6 +1585,7 @@
 values (
 	16,
 	'j.premolo@profesor.duoc.cl',
+	'None',
 	'Premolo',
 	'Yergues',
 	'Juan',
@@ -1501,7 +1595,7 @@
 </v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1509,28 +1603,32 @@
         <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G19" s="1">
-        <v>2</v>
-      </c>
-      <c r="H19" s="3">
-        <v>1</v>
-      </c>
-      <c r="I19" s="2" t="str">
+      <c r="G19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="1">
+        <v>2</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1540,6 +1638,7 @@
 values (
 	17,
 	'car.perezz@profesor.duoc.cl',
+	'None',
 	'Pérez',
 	'Zúñiga',
 	'Carlos',
@@ -1549,7 +1648,7 @@
 </v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1557,28 +1656,32 @@
         <v>42</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G20" s="1">
-        <v>2</v>
-      </c>
-      <c r="H20" s="3">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2" t="str">
+      <c r="G20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1588,6 +1691,7 @@
 values (
 	18,
 	'de.reglas@profesor.duoc.cl',
+	'None',
 	'Reglas',
 	'Villagra',
 	'Deyanira',
@@ -1597,7 +1701,7 @@
 </v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1605,28 +1709,32 @@
         <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21" s="3">
-        <v>2</v>
-      </c>
-      <c r="I21" s="2" t="str">
+      <c r="G21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3">
+        <v>2</v>
+      </c>
+      <c r="J21" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1636,6 +1744,7 @@
 values (
 	19,
 	'dmunita@duoc.cl',
+	'None',
 	'Munita',
 	'Toro',
 	'Daniela',
@@ -1645,7 +1754,7 @@
 </v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1653,28 +1762,32 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="1">
-        <v>2</v>
-      </c>
-      <c r="H22" s="3">
-        <v>2</v>
-      </c>
-      <c r="I22" s="2" t="str">
+      <c r="G22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="1">
+        <v>2</v>
+      </c>
+      <c r="I22" s="3">
+        <v>2</v>
+      </c>
+      <c r="J22" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1684,6 +1797,7 @@
 values (
 	20,
 	'pzamorano@duoc.cl',
+	'None',
 	'Zamorano',
 	'Moreno',
 	'Paola',
@@ -1693,7 +1807,7 @@
 </v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1701,28 +1815,32 @@
         <v>43</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G23" s="1">
-        <v>2</v>
-      </c>
-      <c r="H23" s="3">
-        <v>2</v>
-      </c>
-      <c r="I23" s="2" t="str">
+      <c r="H23" s="1">
+        <v>2</v>
+      </c>
+      <c r="I23" s="3">
+        <v>2</v>
+      </c>
+      <c r="J23" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1732,6 +1850,7 @@
 values (
 	21,
 	'j.enero@profesor.duoc.cl',
+	'None',
 	'Enero',
 	'Rivero',
 	'Juan Francisco',
@@ -1741,7 +1860,7 @@
 </v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1749,28 +1868,32 @@
         <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G24" s="1">
-        <v>2</v>
-      </c>
-      <c r="H24" s="3">
-        <v>2</v>
-      </c>
-      <c r="I24" s="2" t="str">
+      <c r="G24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" s="1">
+        <v>2</v>
+      </c>
+      <c r="I24" s="3">
+        <v>2</v>
+      </c>
+      <c r="J24" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
+	password,
 	primer_apellido,
 	segundo_apellido,
 	nombre,
@@ -1780,6 +1903,7 @@
 values (
 	22,
 	'm.gutierrez2@profesor.duoc.cl',
+	'None',
 	'Gutierrez',
 	'Cortés',
 	'Mauricio',
@@ -1789,14 +1913,14 @@
 </v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J26" t="str">
-        <f t="shared" ref="J26:J27" si="1">LOWER(B26)</f>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K26" t="str">
+        <f t="shared" ref="K26:K27" si="1">LOWER(B26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J27" t="str">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
Correcciones asociadas a la estandarización de las columnas nombre por nom en tabla usuario.
</commit_message>
<xml_diff>
--- a/03 - Base de datos/excel/02 - usuario.xlsx
+++ b/03 - Base de datos/excel/02 - usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Software\Duoc\admtaller-bd\03 - Base de datos\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36F7882-324B-41FA-9EE3-DC30F37913C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B140DC-69AC-47AB-8C03-4F1523B43050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,12 +54,6 @@
     <t>primer_apellido</t>
   </si>
   <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>nombre_preferido</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -319,6 +313,12 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>nom_preferido</t>
   </si>
 </sst>
 </file>
@@ -658,7 +658,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E23" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J24"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -688,19 +688,19 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
@@ -717,19 +717,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
@@ -764,8 +764,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -786,22 +786,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
@@ -836,8 +836,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -858,22 +858,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H5" s="1">
         <v>2</v>
@@ -889,8 +889,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -911,22 +911,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H6" s="1">
         <v>2</v>
@@ -942,8 +942,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -964,22 +964,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H7" s="1">
         <v>2</v>
@@ -995,8 +995,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1017,22 +1017,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H8" s="1">
         <v>2</v>
@@ -1048,8 +1048,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1070,22 +1070,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H9" s="1">
         <v>2</v>
@@ -1101,8 +1101,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1123,22 +1123,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H10" s="1">
         <v>2</v>
@@ -1154,8 +1154,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1176,22 +1176,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H11" s="1">
         <v>2</v>
@@ -1207,8 +1207,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1229,22 +1229,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H12" s="1">
         <v>2</v>
@@ -1260,8 +1260,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1282,22 +1282,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H13" s="1">
         <v>2</v>
@@ -1313,8 +1313,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1335,22 +1335,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H14" s="1">
         <v>2</v>
@@ -1366,8 +1366,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1388,22 +1388,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H15" s="1">
         <v>2</v>
@@ -1419,8 +1419,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1441,22 +1441,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H16" s="1">
         <v>2</v>
@@ -1472,8 +1472,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1494,22 +1494,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H17" s="1">
         <v>2</v>
@@ -1525,8 +1525,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1547,22 +1547,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H18" s="1">
         <v>2</v>
@@ -1578,8 +1578,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1600,22 +1600,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H19" s="1">
         <v>2</v>
@@ -1631,8 +1631,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1653,22 +1653,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H20" s="1">
         <v>2</v>
@@ -1684,8 +1684,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1706,22 +1706,22 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="G21" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H21" s="1">
         <v>1</v>
@@ -1737,8 +1737,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1759,22 +1759,22 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H22" s="1">
         <v>2</v>
@@ -1790,8 +1790,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1812,22 +1812,22 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H23" s="1">
         <v>2</v>
@@ -1843,8 +1843,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (
@@ -1865,22 +1865,22 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="G24" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H24" s="1">
         <v>2</v>
@@ -1896,8 +1896,8 @@
 	password,
 	primer_apellido,
 	segundo_apellido,
-	nombre,
-	nombre_preferido,
+	nom,
+	nom_preferido,
 	cod_perfil,
 	cod_carrera)
 values (

</xml_diff>

<commit_message>
Modificación de estructura de tabla usuario para que se llame hash_password, que sea de 256 caracteres y lo scripts de carga se hace con las claves de los 3 primeros usuarios como es lo usual, para el resto quedó como None aunque por el momento esa funcionalidad falla con usuarios que no están en la lista más que nada porque falla en un servicio simulado que solo considera los 3 primeros.
</commit_message>
<xml_diff>
--- a/03 - Base de datos/excel/02 - usuario.xlsx
+++ b/03 - Base de datos/excel/02 - usuario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Software\Duoc\admtaller-bd\03 - Base de datos\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B140DC-69AC-47AB-8C03-4F1523B43050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0656401A-5EE5-415D-9B27-BB77E194B567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="usuario" sheetId="10" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="105">
   <si>
     <t>tabla</t>
   </si>
@@ -312,20 +312,41 @@
     <t>password</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>nom</t>
   </si>
   <si>
     <t>nom_preferido</t>
+  </si>
+  <si>
+    <t>89b3bd6083da4e8c1b831b66a68a896cf77323a1a615afe859083d2c9ef9b6193e9d48ba4ac55eba00a60b47d967465c96fcc49b5ada64cca3c3fb36b35ac53b</t>
+  </si>
+  <si>
+    <t>274ad1a24014ff7f5102ace0fb916e479dd8900012ccecaf2279ae89b62c2bfbd0cf4b63c2697dbf6cec49cfb2dbcd8d95f0b1021ce70834a3f90bfa467a56f5</t>
+  </si>
+  <si>
+    <t>68dbb47e38b2c86c14ceebea4341b4fbc5aa0ec711a72fdbe7036be1ba93bfd8d2f453e53ef7411a8fabb4f6e5282c3c667d750e0e0e2f47162d7bb6d03a2261</t>
+  </si>
+  <si>
+    <t>6878baad9d3c064fa35754798a445810383a8914080097f9bf57fc69b736b86f19ece34f7f48af0425e6559c3daaec9654c7d8a4edcf80c8e90a336bc61e979a</t>
+  </si>
+  <si>
+    <t>7b0b1427b8a97db8f5c3fa7d2f597e5e836a9f6b9f552f6653ec4c8d29451a7e12af3fe79ae00c0c8a96e2833426b827b7cdaa2a525b59aff8b8f9623c519cbd</t>
+  </si>
+  <si>
+    <t>0b8ad5bf39b2db2a4d54625642d3ef3bff6760794d7d9c5a641888db830479938540f9cc958171af234faac0b67aeb500083ea1d7a6d8c96d107a5b6749fa190</t>
+  </si>
+  <si>
+    <t>2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850</t>
+  </si>
+  <si>
+    <t>admin@duoc.cl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,6 +357,14 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -358,10 +387,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -375,8 +405,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -657,22 +691,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF8A036-CB43-482B-A6BA-E6BCB1927713}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E23" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
-    <col min="4" max="6" width="41.28515625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="39.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="50.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.81640625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="41.26953125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="39.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="50.54296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +714,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -697,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
@@ -712,15 +746,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
+      <c r="B3" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -770,8 +804,8 @@
 	cod_carrera)
 values (
 	1,
-	'admin',
-	'None',
+	'admin@duoc.cl',
+	'89b3bd6083da4e8c1b831b66a68a896cf77323a1a615afe859083d2c9ef9b6193e9d48ba4ac55eba00a60b47d967465c96fcc49b5ada64cca3c3fb36b35ac53b',
 	'Administrador',
 	'',
 	'del sistema',
@@ -781,7 +815,7 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -789,7 +823,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -843,7 +877,7 @@
 values (
 	2,
 	'jmoya@duoc.cl',
-	'None',
+	'274ad1a24014ff7f5102ace0fb916e479dd8900012ccecaf2279ae89b62c2bfbd0cf4b63c2697dbf6cec49cfb2dbcd8d95f0b1021ce70834a3f90bfa467a56f5',
 	'Moya',
 	'Plaza',
 	'Jéssica',
@@ -853,7 +887,7 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -861,7 +895,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -896,7 +930,7 @@
 values (
 	3,
 	'maalvarez@duoc.cl',
-	'None',
+	'68dbb47e38b2c86c14ceebea4341b4fbc5aa0ec711a72fdbe7036be1ba93bfd8d2f453e53ef7411a8fabb4f6e5282c3c667d750e0e0e2f47162d7bb6d03a2261',
 	'Álvarez',
 	'Román',
 	'Marco',
@@ -906,7 +940,7 @@
 </v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -914,7 +948,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>44</v>
@@ -949,7 +983,7 @@
 values (
 	4,
 	'c.gonzalez6@profesor.duoc.cl',
-	'None',
+	'6878baad9d3c064fa35754798a445810383a8914080097f9bf57fc69b736b86f19ece34f7f48af0425e6559c3daaec9654c7d8a4edcf80c8e90a336bc61e979a',
 	'González',
 	'Figueroa',
 	'Cristian',
@@ -959,7 +993,7 @@
 </v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -967,7 +1001,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>47</v>
@@ -1002,7 +1036,7 @@
 values (
 	5,
 	'r.ceura@profesor.duoc.cl',
-	'None',
+	'7b0b1427b8a97db8f5c3fa7d2f597e5e836a9f6b9f552f6653ec4c8d29451a7e12af3fe79ae00c0c8a96e2833426b827b7cdaa2a525b59aff8b8f9623c519cbd',
 	'Ceura',
 	'Vergara',
 	'Raúl',
@@ -1012,7 +1046,7 @@
 </v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1020,7 +1054,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>50</v>
@@ -1055,7 +1089,7 @@
 values (
 	6,
 	'hec.fonseca@profesor.duoc.cl',
-	'None',
+	'0b8ad5bf39b2db2a4d54625642d3ef3bff6760794d7d9c5a641888db830479938540f9cc958171af234faac0b67aeb500083ea1d7a6d8c96d107a5b6749fa190',
 	'Fonseca',
 	'Castillo',
 	'Héctor',
@@ -1065,7 +1099,7 @@
 </v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1073,7 +1107,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>53</v>
@@ -1108,7 +1142,7 @@
 values (
 	7,
 	'xi.castro@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Castro',
 	'Arancibia',
 	'Ximena',
@@ -1118,7 +1152,7 @@
 </v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1126,7 +1160,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>56</v>
@@ -1161,7 +1195,7 @@
 values (
 	8,
 	'c.valenzuelair@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Valenzuela',
 	'Irrazabal',
 	'Carolina',
@@ -1171,7 +1205,7 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1179,7 +1213,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>59</v>
@@ -1214,7 +1248,7 @@
 values (
 	9,
 	'sa.navarret@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Navarrete',
 	'Bustamante',
 	'Sandra',
@@ -1224,7 +1258,7 @@
 </v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1232,7 +1266,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>54</v>
@@ -1267,7 +1301,7 @@
 values (
 	10,
 	'fabi.arancibia@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Arancibia',
 	'Severino',
 	'Fabián',
@@ -1277,7 +1311,7 @@
 </v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1285,7 +1319,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>63</v>
@@ -1320,7 +1354,7 @@
 values (
 	11,
 	'roci.guzman@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Guzmán',
 	'Acuña',
 	'Rocío',
@@ -1330,7 +1364,7 @@
 </v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1338,7 +1372,7 @@
         <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>66</v>
@@ -1373,7 +1407,7 @@
 values (
 	12,
 	'al.camposa@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Campos',
 	'Acuña',
 	'Alejandra',
@@ -1383,7 +1417,7 @@
 </v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1391,7 +1425,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>68</v>
@@ -1426,7 +1460,7 @@
 values (
 	13,
 	'cr.madariagam@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Madariaga',
 	'Martínez',
 	'Cristian',
@@ -1436,7 +1470,7 @@
 </v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1444,7 +1478,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>70</v>
@@ -1479,7 +1513,7 @@
 values (
 	14,
 	'i.inostroza@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Inostroza',
 	'Rodríguez',
 	'Isaac',
@@ -1489,7 +1523,7 @@
 </v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1497,7 +1531,7 @@
         <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>73</v>
@@ -1532,7 +1566,7 @@
 values (
 	15,
 	'v.fuentealbav@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Fuentealva',
 	'Vargas',
 	'Víctor',
@@ -1542,7 +1576,7 @@
 </v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1550,7 +1584,7 @@
         <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>76</v>
@@ -1585,7 +1619,7 @@
 values (
 	16,
 	'j.premolo@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Premolo',
 	'Yergues',
 	'Juan',
@@ -1595,7 +1629,7 @@
 </v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1603,7 +1637,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>79</v>
@@ -1638,7 +1672,7 @@
 values (
 	17,
 	'car.perezz@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Pérez',
 	'Zúñiga',
 	'Carlos',
@@ -1648,7 +1682,7 @@
 </v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1656,7 +1690,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>82</v>
@@ -1691,7 +1725,7 @@
 values (
 	18,
 	'de.reglas@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Reglas',
 	'Villagra',
 	'Deyanira',
@@ -1701,7 +1735,7 @@
 </v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1709,7 +1743,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>15</v>
@@ -1744,7 +1778,7 @@
 values (
 	19,
 	'dmunita@duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Munita',
 	'Toro',
 	'Daniela',
@@ -1754,7 +1788,7 @@
 </v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1762,7 +1796,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>20</v>
@@ -1797,7 +1831,7 @@
 values (
 	20,
 	'pzamorano@duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Zamorano',
 	'Moreno',
 	'Paola',
@@ -1807,7 +1841,7 @@
 </v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1815,7 +1849,7 @@
         <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>87</v>
@@ -1850,7 +1884,7 @@
 values (
 	21,
 	'j.enero@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Enero',
 	'Rivero',
 	'Juan Francisco',
@@ -1860,7 +1894,7 @@
 </v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1868,7 +1902,7 @@
         <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>90</v>
@@ -1903,7 +1937,7 @@
 values (
 	22,
 	'm.gutierrez2@profesor.duoc.cl',
-	'None',
+	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
 	'Gutierrez',
 	'Cortés',
 	'Mauricio',
@@ -1913,19 +1947,22 @@
 </v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K26" t="str">
         <f t="shared" ref="K26:K27" si="1">LOWER(B26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{C6159219-12DB-4639-ABAA-36EEA1A475E7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correcciones a la contraseña encriptada de los usuarios distintos al 1, 2 y 3. Queda como None.
</commit_message>
<xml_diff>
--- a/03 - Base de datos/excel/02 - usuario.xlsx
+++ b/03 - Base de datos/excel/02 - usuario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Software\Duoc\admtaller-bd\03 - Base de datos\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0656401A-5EE5-415D-9B27-BB77E194B567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E2AC23-00DC-4FB2-A826-9D96BA021CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="usuario" sheetId="10" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="102">
   <si>
     <t>tabla</t>
   </si>
@@ -309,9 +309,6 @@
     <t>Fabián</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>nom</t>
   </si>
   <si>
@@ -327,19 +324,13 @@
     <t>68dbb47e38b2c86c14ceebea4341b4fbc5aa0ec711a72fdbe7036be1ba93bfd8d2f453e53ef7411a8fabb4f6e5282c3c667d750e0e0e2f47162d7bb6d03a2261</t>
   </si>
   <si>
-    <t>6878baad9d3c064fa35754798a445810383a8914080097f9bf57fc69b736b86f19ece34f7f48af0425e6559c3daaec9654c7d8a4edcf80c8e90a336bc61e979a</t>
-  </si>
-  <si>
-    <t>7b0b1427b8a97db8f5c3fa7d2f597e5e836a9f6b9f552f6653ec4c8d29451a7e12af3fe79ae00c0c8a96e2833426b827b7cdaa2a525b59aff8b8f9623c519cbd</t>
-  </si>
-  <si>
-    <t>0b8ad5bf39b2db2a4d54625642d3ef3bff6760794d7d9c5a641888db830479938540f9cc958171af234faac0b67aeb500083ea1d7a6d8c96d107a5b6749fa190</t>
-  </si>
-  <si>
-    <t>2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850</t>
-  </si>
-  <si>
     <t>admin@duoc.cl</t>
+  </si>
+  <si>
+    <t>dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0</t>
+  </si>
+  <si>
+    <t>hash_password</t>
   </si>
 </sst>
 </file>
@@ -691,22 +682,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF8A036-CB43-482B-A6BA-E6BCB1927713}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.81640625" style="1" customWidth="1"/>
-    <col min="4" max="6" width="41.26953125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="39.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="50.54296875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
+    <col min="4" max="6" width="41.28515625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="39.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="50.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,7 +705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -722,7 +713,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -731,10 +722,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
@@ -746,15 +737,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -795,7 +786,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -815,7 +806,7 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -823,7 +814,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -867,7 +858,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -887,7 +878,7 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -895,7 +886,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -920,7 +911,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -940,7 +931,7 @@
 </v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -973,7 +964,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -983,7 +974,7 @@
 values (
 	4,
 	'c.gonzalez6@profesor.duoc.cl',
-	'6878baad9d3c064fa35754798a445810383a8914080097f9bf57fc69b736b86f19ece34f7f48af0425e6559c3daaec9654c7d8a4edcf80c8e90a336bc61e979a',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'González',
 	'Figueroa',
 	'Cristian',
@@ -993,7 +984,7 @@
 </v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1001,7 +992,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>47</v>
@@ -1026,7 +1017,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1036,7 +1027,7 @@
 values (
 	5,
 	'r.ceura@profesor.duoc.cl',
-	'7b0b1427b8a97db8f5c3fa7d2f597e5e836a9f6b9f552f6653ec4c8d29451a7e12af3fe79ae00c0c8a96e2833426b827b7cdaa2a525b59aff8b8f9623c519cbd',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Ceura',
 	'Vergara',
 	'Raúl',
@@ -1046,7 +1037,7 @@
 </v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1054,7 +1045,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>50</v>
@@ -1079,7 +1070,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1089,7 +1080,7 @@
 values (
 	6,
 	'hec.fonseca@profesor.duoc.cl',
-	'0b8ad5bf39b2db2a4d54625642d3ef3bff6760794d7d9c5a641888db830479938540f9cc958171af234faac0b67aeb500083ea1d7a6d8c96d107a5b6749fa190',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Fonseca',
 	'Castillo',
 	'Héctor',
@@ -1099,7 +1090,7 @@
 </v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1107,7 +1098,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>53</v>
@@ -1132,7 +1123,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1142,7 +1133,7 @@
 values (
 	7,
 	'xi.castro@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Castro',
 	'Arancibia',
 	'Ximena',
@@ -1152,7 +1143,7 @@
 </v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1160,7 +1151,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>56</v>
@@ -1185,7 +1176,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1195,7 +1186,7 @@
 values (
 	8,
 	'c.valenzuelair@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Valenzuela',
 	'Irrazabal',
 	'Carolina',
@@ -1205,7 +1196,7 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1213,7 +1204,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>59</v>
@@ -1238,7 +1229,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1248,7 +1239,7 @@
 values (
 	9,
 	'sa.navarret@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Navarrete',
 	'Bustamante',
 	'Sandra',
@@ -1258,7 +1249,7 @@
 </v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1266,7 +1257,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>54</v>
@@ -1291,7 +1282,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1301,7 +1292,7 @@
 values (
 	10,
 	'fabi.arancibia@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Arancibia',
 	'Severino',
 	'Fabián',
@@ -1311,7 +1302,7 @@
 </v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1319,7 +1310,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>63</v>
@@ -1344,7 +1335,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1354,7 +1345,7 @@
 values (
 	11,
 	'roci.guzman@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Guzmán',
 	'Acuña',
 	'Rocío',
@@ -1364,7 +1355,7 @@
 </v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1372,7 +1363,7 @@
         <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>66</v>
@@ -1397,7 +1388,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1407,7 +1398,7 @@
 values (
 	12,
 	'al.camposa@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Campos',
 	'Acuña',
 	'Alejandra',
@@ -1417,7 +1408,7 @@
 </v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1425,7 +1416,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>68</v>
@@ -1450,7 +1441,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1460,7 +1451,7 @@
 values (
 	13,
 	'cr.madariagam@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Madariaga',
 	'Martínez',
 	'Cristian',
@@ -1470,7 +1461,7 @@
 </v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1478,7 +1469,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>70</v>
@@ -1503,7 +1494,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1513,7 +1504,7 @@
 values (
 	14,
 	'i.inostroza@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Inostroza',
 	'Rodríguez',
 	'Isaac',
@@ -1523,7 +1514,7 @@
 </v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1531,7 +1522,7 @@
         <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>73</v>
@@ -1556,7 +1547,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1566,7 +1557,7 @@
 values (
 	15,
 	'v.fuentealbav@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Fuentealva',
 	'Vargas',
 	'Víctor',
@@ -1576,7 +1567,7 @@
 </v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1584,7 +1575,7 @@
         <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>76</v>
@@ -1609,7 +1600,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1619,7 +1610,7 @@
 values (
 	16,
 	'j.premolo@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Premolo',
 	'Yergues',
 	'Juan',
@@ -1629,7 +1620,7 @@
 </v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1637,7 +1628,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>79</v>
@@ -1662,7 +1653,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1672,7 +1663,7 @@
 values (
 	17,
 	'car.perezz@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Pérez',
 	'Zúñiga',
 	'Carlos',
@@ -1682,7 +1673,7 @@
 </v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1690,7 +1681,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>82</v>
@@ -1715,7 +1706,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1725,7 +1716,7 @@
 values (
 	18,
 	'de.reglas@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Reglas',
 	'Villagra',
 	'Deyanira',
@@ -1735,7 +1726,7 @@
 </v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1743,7 +1734,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>15</v>
@@ -1768,7 +1759,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1778,7 +1769,7 @@
 values (
 	19,
 	'dmunita@duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Munita',
 	'Toro',
 	'Daniela',
@@ -1788,7 +1779,7 @@
 </v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1796,7 +1787,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>20</v>
@@ -1821,7 +1812,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1831,7 +1822,7 @@
 values (
 	20,
 	'pzamorano@duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Zamorano',
 	'Moreno',
 	'Paola',
@@ -1841,7 +1832,7 @@
 </v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1849,7 +1840,7 @@
         <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>87</v>
@@ -1874,7 +1865,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1884,7 +1875,7 @@
 values (
 	21,
 	'j.enero@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Enero',
 	'Rivero',
 	'Juan Francisco',
@@ -1894,7 +1885,7 @@
 </v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="220.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1902,7 +1893,7 @@
         <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>90</v>
@@ -1927,7 +1918,7 @@
         <v xml:space="preserve">insert into usuario (
 	id_usuario,
 	login,
-	password,
+	hash_password,
 	primer_apellido,
 	segundo_apellido,
 	nom,
@@ -1937,7 +1928,7 @@
 values (
 	22,
 	'm.gutierrez2@profesor.duoc.cl',
-	'2a911471076d524988bf8512f67c215bbec5a40de9dd4ef2c2fd5c3d6cca2b4e12408b796498c28f052b922599b9afe6aa499062b00cf620d3bcab5ac3bbd850',
+	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Gutierrez',
 	'Cortés',
 	'Mauricio',
@@ -1947,13 +1938,13 @@
 </v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K26" t="str">
         <f t="shared" ref="K26:K27" si="1">LOWER(B26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K27" t="str">
         <f t="shared" si="1"/>
         <v/>

</xml_diff>

<commit_message>
Se corrige apellido de Fuentealba.
</commit_message>
<xml_diff>
--- a/03 - Base de datos/excel/02 - usuario.xlsx
+++ b/03 - Base de datos/excel/02 - usuario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Software\Duoc\admtaller-bd\03 - Base de datos\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E2AC23-00DC-4FB2-A826-9D96BA021CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D815877E-881B-4686-89D5-CF5979114BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="usuario" sheetId="10" r:id="rId1"/>
@@ -246,9 +246,6 @@
     <t>Isaac</t>
   </si>
   <si>
-    <t>Fuentealva</t>
-  </si>
-  <si>
     <t>Vargas</t>
   </si>
   <si>
@@ -331,6 +328,9 @@
   </si>
   <si>
     <t>hash_password</t>
+  </si>
+  <si>
+    <t>Fuentealba</t>
   </si>
 </sst>
 </file>
@@ -682,22 +682,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF8A036-CB43-482B-A6BA-E6BCB1927713}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
-    <col min="4" max="6" width="41.28515625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="39.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="50.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.81640625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="41.26953125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="39.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="50.54296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,7 +705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -713,7 +713,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -722,10 +722,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
@@ -737,15 +737,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -806,7 +806,7 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -814,7 +814,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -878,7 +878,7 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -886,7 +886,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -931,7 +931,7 @@
 </v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -939,7 +939,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>44</v>
@@ -984,7 +984,7 @@
 </v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -992,7 +992,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>47</v>
@@ -1037,7 +1037,7 @@
 </v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>50</v>
@@ -1090,7 +1090,7 @@
 </v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>53</v>
@@ -1143,7 +1143,7 @@
 </v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>56</v>
@@ -1196,7 +1196,7 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>59</v>
@@ -1249,7 +1249,7 @@
 </v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>54</v>
@@ -1266,10 +1266,10 @@
         <v>62</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H12" s="1">
         <v>2</v>
@@ -1302,7 +1302,7 @@
 </v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>63</v>
@@ -1355,7 +1355,7 @@
 </v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>66</v>
@@ -1408,7 +1408,7 @@
 </v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>68</v>
@@ -1461,7 +1461,7 @@
 </v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="231" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>70</v>
@@ -1514,7 +1514,7 @@
 </v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="231" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1522,19 +1522,19 @@
         <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H17" s="1">
         <v>2</v>
@@ -1558,7 +1558,7 @@
 	15,
 	'v.fuentealbav@profesor.duoc.cl',
 	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
-	'Fuentealva',
+	'Fuentealba',
 	'Vargas',
 	'Víctor',
 	'Víctor',
@@ -1567,7 +1567,7 @@
 </v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="231" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1575,19 +1575,19 @@
         <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H18" s="1">
         <v>2</v>
@@ -1620,7 +1620,7 @@
 </v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="231" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1628,19 +1628,19 @@
         <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H19" s="1">
         <v>2</v>
@@ -1673,7 +1673,7 @@
 </v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="231" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1681,19 +1681,19 @@
         <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H20" s="1">
         <v>2</v>
@@ -1726,7 +1726,7 @@
 </v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="231" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1734,13 +1734,13 @@
         <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>16</v>
@@ -1779,7 +1779,7 @@
 </v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="231" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1787,13 +1787,13 @@
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>21</v>
@@ -1832,7 +1832,7 @@
 </v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="231" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1840,19 +1840,19 @@
         <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H23" s="1">
         <v>2</v>
@@ -1885,7 +1885,7 @@
 </v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="231" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1893,19 +1893,19 @@
         <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="G24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H24" s="1">
         <v>2</v>
@@ -1938,13 +1938,13 @@
 </v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K26" t="str">
         <f t="shared" ref="K26:K27" si="1">LOWER(B26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K27" t="str">
         <f t="shared" si="1"/>
         <v/>

</xml_diff>

<commit_message>
Correcciones a scripts para datos de prueba.
</commit_message>
<xml_diff>
--- a/03 - Base de datos/excel/02 - usuario.xlsx
+++ b/03 - Base de datos/excel/02 - usuario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Software\Duoc\admtaller-bd\03 - Base de datos\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D815877E-881B-4686-89D5-CF5979114BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61A85F6-58EB-4FEB-B233-4E990EAF0171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="usuario" sheetId="10" r:id="rId1"/>
@@ -198,9 +198,6 @@
     <t>Valenzuela</t>
   </si>
   <si>
-    <t>Irrazabal</t>
-  </si>
-  <si>
     <t>Carolina</t>
   </si>
   <si>
@@ -252,9 +249,6 @@
     <t>Víctor</t>
   </si>
   <si>
-    <t>Premolo</t>
-  </si>
-  <si>
     <t>Yergues</t>
   </si>
   <si>
@@ -294,9 +288,6 @@
     <t>Juan Francisco</t>
   </si>
   <si>
-    <t>Gutierrez</t>
-  </si>
-  <si>
     <t>Cortés</t>
   </si>
   <si>
@@ -312,9 +303,6 @@
     <t>nom_preferido</t>
   </si>
   <si>
-    <t>89b3bd6083da4e8c1b831b66a68a896cf77323a1a615afe859083d2c9ef9b6193e9d48ba4ac55eba00a60b47d967465c96fcc49b5ada64cca3c3fb36b35ac53b</t>
-  </si>
-  <si>
     <t>274ad1a24014ff7f5102ace0fb916e479dd8900012ccecaf2279ae89b62c2bfbd0cf4b63c2697dbf6cec49cfb2dbcd8d95f0b1021ce70834a3f90bfa467a56f5</t>
   </si>
   <si>
@@ -331,6 +319,18 @@
   </si>
   <si>
     <t>Fuentealba</t>
+  </si>
+  <si>
+    <t>Irrázabal</t>
+  </si>
+  <si>
+    <t>Prémolo</t>
+  </si>
+  <si>
+    <t>Gutiérrez</t>
+  </si>
+  <si>
+    <t>c16fd958b85a1c94d872c219ea06ce8e80223239b1fcefb92ad978445ef095507244be44caae1d766e277b072c184cb3ffe4d0610716e989b2fe5a7c97bf3144</t>
   </si>
 </sst>
 </file>
@@ -682,22 +682,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF8A036-CB43-482B-A6BA-E6BCB1927713}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.81640625" style="1" customWidth="1"/>
-    <col min="4" max="6" width="41.26953125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="39.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="50.54296875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
+    <col min="4" max="6" width="41.28515625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="39.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="50.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,7 +705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -713,7 +713,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -722,10 +722,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
@@ -737,15 +737,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -796,7 +796,7 @@
 values (
 	1,
 	'admin@duoc.cl',
-	'89b3bd6083da4e8c1b831b66a68a896cf77323a1a615afe859083d2c9ef9b6193e9d48ba4ac55eba00a60b47d967465c96fcc49b5ada64cca3c3fb36b35ac53b',
+	'c16fd958b85a1c94d872c219ea06ce8e80223239b1fcefb92ad978445ef095507244be44caae1d766e277b072c184cb3ffe4d0610716e989b2fe5a7c97bf3144',
 	'Administrador',
 	'',
 	'del sistema',
@@ -806,7 +806,7 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -814,7 +814,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -878,7 +878,7 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -886,7 +886,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -931,7 +931,7 @@
 </v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -939,7 +939,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>44</v>
@@ -984,7 +984,7 @@
 </v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -992,7 +992,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>47</v>
@@ -1037,7 +1037,7 @@
 </v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>50</v>
@@ -1090,7 +1090,7 @@
 </v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>53</v>
@@ -1143,7 +1143,7 @@
 </v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1151,19 +1151,19 @@
         <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H10" s="1">
         <v>2</v>
@@ -1188,7 +1188,7 @@
 	'c.valenzuelair@profesor.duoc.cl',
 	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
 	'Valenzuela',
-	'Irrazabal',
+	'Irrázabal',
 	'Carolina',
 	'Carolina',
 	2,
@@ -1196,7 +1196,7 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1204,19 +1204,19 @@
         <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H11" s="1">
         <v>2</v>
@@ -1249,7 +1249,7 @@
 </v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1257,19 +1257,19 @@
         <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H12" s="1">
         <v>2</v>
@@ -1302,7 +1302,7 @@
 </v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1310,19 +1310,19 @@
         <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H13" s="1">
         <v>2</v>
@@ -1355,7 +1355,7 @@
 </v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1363,19 +1363,19 @@
         <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H14" s="1">
         <v>2</v>
@@ -1408,7 +1408,7 @@
 </v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1416,13 +1416,13 @@
         <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>46</v>
@@ -1461,7 +1461,7 @@
 </v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1469,19 +1469,19 @@
         <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H16" s="1">
         <v>2</v>
@@ -1514,7 +1514,7 @@
 </v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="231" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1522,19 +1522,19 @@
         <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H17" s="1">
         <v>2</v>
@@ -1567,7 +1567,7 @@
 </v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="231" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1575,19 +1575,19 @@
         <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H18" s="1">
         <v>2</v>
@@ -1611,7 +1611,7 @@
 	16,
 	'j.premolo@profesor.duoc.cl',
 	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
-	'Premolo',
+	'Prémolo',
 	'Yergues',
 	'Juan',
 	'Juan',
@@ -1620,7 +1620,7 @@
 </v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="231" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1628,19 +1628,19 @@
         <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H19" s="1">
         <v>2</v>
@@ -1673,7 +1673,7 @@
 </v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="231" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1681,19 +1681,19 @@
         <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H20" s="1">
         <v>2</v>
@@ -1726,7 +1726,7 @@
 </v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="231" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1734,13 +1734,13 @@
         <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>16</v>
@@ -1779,7 +1779,7 @@
 </v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="231" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1787,13 +1787,13 @@
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>21</v>
@@ -1832,7 +1832,7 @@
 </v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="231" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1840,19 +1840,19 @@
         <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H23" s="1">
         <v>2</v>
@@ -1885,7 +1885,7 @@
 </v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="231" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1893,19 +1893,19 @@
         <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H24" s="1">
         <v>2</v>
@@ -1929,7 +1929,7 @@
 	22,
 	'm.gutierrez2@profesor.duoc.cl',
 	'dbb8d24a3166d17cd46539f4dca51ac945174b0ed8491859f690ddb24fe6cb74fbbf3338766d273903b8748da32c5a9c645ff0a2013c7412edc38b64cf8f2ec0',
-	'Gutierrez',
+	'Gutiérrez',
 	'Cortés',
 	'Mauricio',
 	'Mauricio',
@@ -1938,13 +1938,13 @@
 </v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K26" t="str">
         <f t="shared" ref="K26:K27" si="1">LOWER(B26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K27" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -1955,5 +1955,6 @@
     <hyperlink ref="B3" r:id="rId1" xr:uid="{C6159219-12DB-4639-ABAA-36EEA1A475E7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>